<commit_message>
proyecto funcional y culminando
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/DOCUMENTOS/Matriz Requisitos.xlsx
+++ b/DOCUMENTACION/DOCUMENTOS/Matriz Requisitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Repositorio Colegio Pereira\DOCUMENTACION\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F15FB6-04B9-447D-B289-925C75C2DC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D99F664-FF47-40D2-AB90-D548C0166BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RF" sheetId="1" r:id="rId1"/>
@@ -1864,7 +1864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1954,14 +1954,153 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2006,6 +2145,47 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2018,12 +2198,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2031,7 +2210,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2041,7 +2219,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2095,192 +2272,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2708,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2728,100 +2719,100 @@
   <sheetData>
     <row r="1" spans="1:13" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="38" t="s">
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="39"/>
+      <c r="I2" s="84"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="45"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="86"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="45"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="86"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="45"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="86"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="46"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="88"/>
     </row>
     <row r="7" spans="1:13" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="50" t="s">
+      <c r="E8" s="97"/>
+      <c r="F8" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="50" t="s">
+      <c r="G8" s="97"/>
+      <c r="H8" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="51"/>
+      <c r="I8" s="96"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="99"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="101"/>
       <c r="D9" s="28" t="s">
         <v>20</v>
       </c>
@@ -2846,28 +2837,28 @@
     </row>
     <row r="10" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="135" t="s">
+      <c r="B10" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="133" t="s">
+      <c r="C10" s="34" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="123" t="s">
+      <c r="E10" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="145" t="s">
+      <c r="F10" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="150" t="s">
+      <c r="G10" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="H10" s="145" t="s">
+      <c r="H10" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="148" t="s">
+      <c r="I10" s="66" t="s">
         <v>166</v>
       </c>
       <c r="J10" s="1"/>
@@ -2876,26 +2867,26 @@
     </row>
     <row r="11" spans="1:13" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="136"/>
-      <c r="C11" s="134" t="s">
+      <c r="B11" s="103"/>
+      <c r="C11" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="124" t="s">
+      <c r="E11" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="146" t="s">
+      <c r="F11" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="151" t="s">
+      <c r="G11" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="H11" s="145" t="s">
+      <c r="H11" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="I11" s="147" t="s">
+      <c r="I11" s="65" t="s">
         <v>170</v>
       </c>
       <c r="J11" s="1"/>
@@ -2904,28 +2895,28 @@
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="119" t="s">
+      <c r="B12" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="101" t="s">
+      <c r="D12" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="125" t="s">
+      <c r="E12" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="145" t="s">
+      <c r="F12" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="152" t="s">
+      <c r="G12" s="70" t="s">
         <v>169</v>
       </c>
-      <c r="H12" s="145" t="s">
+      <c r="H12" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="I12" s="147" t="s">
+      <c r="I12" s="65" t="s">
         <v>168</v>
       </c>
       <c r="J12" s="1"/>
@@ -2934,22 +2925,22 @@
     </row>
     <row r="13" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="119"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="101" t="s">
+      <c r="B13" s="106"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="126" t="s">
+      <c r="E13" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="146" t="s">
+      <c r="F13" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="G13" s="149"/>
-      <c r="H13" s="145" t="s">
+      <c r="G13" s="67"/>
+      <c r="H13" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="I13" s="147" t="s">
+      <c r="I13" s="65" t="s">
         <v>171</v>
       </c>
       <c r="J13" s="1"/>
@@ -2959,26 +2950,26 @@
     </row>
     <row r="14" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="106"/>
+      <c r="C14" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="101" t="s">
+      <c r="D14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="125" t="s">
+      <c r="E14" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="145" t="s">
+      <c r="F14" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="153" t="s">
+      <c r="G14" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="H14" s="145" t="s">
+      <c r="H14" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="I14" s="147" t="s">
+      <c r="I14" s="65" t="s">
         <v>173</v>
       </c>
       <c r="J14" s="1"/>
@@ -2987,24 +2978,24 @@
     </row>
     <row r="15" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="120"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="101" t="s">
+      <c r="B15" s="107"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="126" t="s">
+      <c r="E15" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="146" t="s">
+      <c r="F15" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="G15" s="153" t="s">
+      <c r="G15" s="71" t="s">
         <v>188</v>
       </c>
-      <c r="H15" s="145" t="s">
+      <c r="H15" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="I15" s="154" t="s">
+      <c r="I15" s="72" t="s">
         <v>174</v>
       </c>
       <c r="J15" s="1"/>
@@ -3013,26 +3004,26 @@
     </row>
     <row r="16" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="137" t="s">
+      <c r="B16" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="101" t="s">
+      <c r="D16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="125" t="s">
+      <c r="E16" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="145" t="s">
+      <c r="F16" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="153"/>
-      <c r="H16" s="145" t="s">
+      <c r="G16" s="71"/>
+      <c r="H16" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="I16" s="154" t="s">
+      <c r="I16" s="72" t="s">
         <v>176</v>
       </c>
       <c r="J16" s="1"/>
@@ -3041,22 +3032,22 @@
     </row>
     <row r="17" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="137"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="101" t="s">
+      <c r="B17" s="80"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="126" t="s">
+      <c r="E17" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="146" t="s">
+      <c r="F17" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="G17" s="153"/>
-      <c r="H17" s="145" t="s">
+      <c r="G17" s="71"/>
+      <c r="H17" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="I17" s="154" t="s">
+      <c r="I17" s="72" t="s">
         <v>175</v>
       </c>
       <c r="J17" s="1"/>
@@ -3065,46 +3056,45 @@
     </row>
     <row r="18" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="137"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="101" t="s">
+      <c r="B18" s="80"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="127" t="s">
+      <c r="E18" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="145" t="s">
+      <c r="F18" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="G18" s="109"/>
-      <c r="H18" s="145" t="s">
+      <c r="H18" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="155"/>
+      <c r="I18" s="73"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="137"/>
-      <c r="C19" s="139" t="s">
+      <c r="B19" s="80"/>
+      <c r="C19" s="78" t="s">
         <v>82</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="128" t="s">
+      <c r="E19" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="146" t="s">
+      <c r="F19" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="153"/>
-      <c r="H19" s="145" t="s">
+      <c r="G19" s="71"/>
+      <c r="H19" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="I19" s="154" t="s">
+      <c r="I19" s="72" t="s">
         <v>177</v>
       </c>
       <c r="J19" s="1"/>
@@ -3113,22 +3103,22 @@
     </row>
     <row r="20" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="137"/>
-      <c r="C20" s="140"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="128" t="s">
+      <c r="E20" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="145" t="s">
+      <c r="F20" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="G20" s="153"/>
-      <c r="H20" s="145" t="s">
+      <c r="G20" s="71"/>
+      <c r="H20" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="I20" s="154" t="s">
+      <c r="I20" s="72" t="s">
         <v>178</v>
       </c>
       <c r="J20" s="1"/>
@@ -3137,22 +3127,22 @@
     </row>
     <row r="21" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="137"/>
-      <c r="C21" s="140"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="128" t="s">
+      <c r="E21" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="146" t="s">
+      <c r="F21" s="64" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="153"/>
-      <c r="H21" s="145" t="s">
+      <c r="G21" s="71"/>
+      <c r="H21" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="I21" s="154" t="s">
+      <c r="I21" s="72" t="s">
         <v>179</v>
       </c>
       <c r="J21" s="1"/>
@@ -3161,22 +3151,22 @@
     </row>
     <row r="22" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="137"/>
-      <c r="C22" s="140"/>
-      <c r="D22" s="97" t="s">
+      <c r="B22" s="80"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="128" t="s">
+      <c r="E22" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="145" t="s">
+      <c r="F22" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="153"/>
-      <c r="H22" s="145" t="s">
+      <c r="G22" s="71"/>
+      <c r="H22" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="I22" s="154" t="s">
+      <c r="I22" s="72" t="s">
         <v>180</v>
       </c>
       <c r="J22" s="1"/>
@@ -3185,22 +3175,22 @@
     </row>
     <row r="23" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="137"/>
-      <c r="C23" s="140"/>
-      <c r="D23" s="101" t="s">
+      <c r="B23" s="80"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="128" t="s">
+      <c r="E23" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="146" t="s">
+      <c r="F23" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="G23" s="153"/>
-      <c r="H23" s="145" t="s">
+      <c r="G23" s="71"/>
+      <c r="H23" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="I23" s="154" t="s">
+      <c r="I23" s="72" t="s">
         <v>181</v>
       </c>
       <c r="J23" s="1"/>
@@ -3209,22 +3199,22 @@
     </row>
     <row r="24" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="137"/>
-      <c r="C24" s="140"/>
-      <c r="D24" s="101" t="s">
+      <c r="B24" s="80"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="128" t="s">
+      <c r="E24" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="145" t="s">
+      <c r="F24" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="153"/>
-      <c r="H24" s="145" t="s">
+      <c r="G24" s="71"/>
+      <c r="H24" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="I24" s="154" t="s">
+      <c r="I24" s="72" t="s">
         <v>182</v>
       </c>
       <c r="J24" s="1"/>
@@ -3233,24 +3223,24 @@
     </row>
     <row r="25" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="137"/>
-      <c r="C25" s="140"/>
-      <c r="D25" s="101" t="s">
+      <c r="B25" s="80"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="128" t="s">
+      <c r="E25" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="146" t="s">
+      <c r="F25" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="153" t="s">
+      <c r="G25" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="H25" s="145" t="s">
+      <c r="H25" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="I25" s="154" t="s">
+      <c r="I25" s="72" t="s">
         <v>183</v>
       </c>
       <c r="J25" s="1"/>
@@ -3259,44 +3249,44 @@
     </row>
     <row r="26" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="137"/>
-      <c r="C26" s="140"/>
-      <c r="D26" s="101" t="s">
+      <c r="B26" s="80"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="128" t="s">
+      <c r="E26" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="F26" s="145" t="s">
+      <c r="F26" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="153"/>
-      <c r="H26" s="145" t="s">
+      <c r="G26" s="71"/>
+      <c r="H26" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="I26" s="154"/>
+      <c r="I26" s="72"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="137"/>
-      <c r="C27" s="140"/>
-      <c r="D27" s="101" t="s">
+      <c r="B27" s="80"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="128" t="s">
+      <c r="E27" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="146" t="s">
+      <c r="F27" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="153"/>
-      <c r="H27" s="145" t="s">
+      <c r="G27" s="71"/>
+      <c r="H27" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="I27" s="154" t="s">
+      <c r="I27" s="72" t="s">
         <v>180</v>
       </c>
       <c r="J27" s="1"/>
@@ -3305,136 +3295,136 @@
     </row>
     <row r="28" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="137"/>
-      <c r="C28" s="140"/>
-      <c r="D28" s="101" t="s">
+      <c r="B28" s="80"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="129" t="s">
+      <c r="E28" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="145" t="s">
+      <c r="F28" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="G28" s="153"/>
-      <c r="H28" s="145" t="s">
+      <c r="G28" s="71"/>
+      <c r="H28" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="I28" s="154"/>
+      <c r="I28" s="72"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="137"/>
-      <c r="C29" s="140"/>
-      <c r="D29" s="101" t="s">
+      <c r="B29" s="80"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="128" t="s">
+      <c r="E29" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="146" t="s">
+      <c r="F29" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="G29" s="153"/>
-      <c r="H29" s="145" t="s">
+      <c r="G29" s="71"/>
+      <c r="H29" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="I29" s="154"/>
+      <c r="I29" s="72"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="137"/>
-      <c r="C30" s="140"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="79"/>
       <c r="D30" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="126" t="s">
+      <c r="E30" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="145" t="s">
+      <c r="F30" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G30" s="153"/>
-      <c r="H30" s="145" t="s">
+      <c r="G30" s="71"/>
+      <c r="H30" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="I30" s="154"/>
+      <c r="I30" s="72"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
     <row r="31" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="137"/>
-      <c r="C31" s="140"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="126" t="s">
+      <c r="E31" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="F31" s="146" t="s">
+      <c r="F31" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="G31" s="153"/>
-      <c r="H31" s="145" t="s">
+      <c r="G31" s="71"/>
+      <c r="H31" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="I31" s="154"/>
+      <c r="I31" s="72"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="137"/>
-      <c r="C32" s="140"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="79"/>
       <c r="D32" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="130" t="s">
+      <c r="E32" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="145" t="s">
+      <c r="F32" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="G32" s="153" t="s">
+      <c r="G32" s="71" t="s">
         <v>193</v>
       </c>
-      <c r="H32" s="145" t="s">
+      <c r="H32" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="I32" s="154"/>
+      <c r="I32" s="72"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="137"/>
-      <c r="C33" s="138" t="s">
+      <c r="B33" s="80"/>
+      <c r="C33" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="97" t="s">
+      <c r="D33" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="128" t="s">
+      <c r="E33" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="F33" s="146" t="s">
+      <c r="F33" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="G33" s="153"/>
-      <c r="H33" s="145" t="s">
+      <c r="G33" s="71"/>
+      <c r="H33" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="I33" s="154" t="s">
+      <c r="I33" s="72" t="s">
         <v>184</v>
       </c>
       <c r="J33" s="1"/>
@@ -3443,24 +3433,24 @@
     </row>
     <row r="34" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="137"/>
-      <c r="C34" s="138"/>
-      <c r="D34" s="108" t="s">
+      <c r="B34" s="80"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="128" t="s">
+      <c r="E34" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="145" t="s">
+      <c r="F34" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="G34" s="153" t="s">
+      <c r="G34" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="H34" s="145" t="s">
+      <c r="H34" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="I34" s="154" t="s">
+      <c r="I34" s="72" t="s">
         <v>185</v>
       </c>
       <c r="J34" s="1"/>
@@ -3469,24 +3459,24 @@
     </row>
     <row r="35" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="137"/>
-      <c r="C35" s="132" t="s">
+      <c r="B35" s="80"/>
+      <c r="C35" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="107" t="s">
+      <c r="D35" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="122" t="s">
+      <c r="E35" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="146" t="s">
+      <c r="F35" s="64" t="s">
         <v>133</v>
       </c>
-      <c r="G35" s="153"/>
-      <c r="H35" s="145" t="s">
+      <c r="G35" s="71"/>
+      <c r="H35" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="I35" s="147" t="s">
+      <c r="I35" s="65" t="s">
         <v>186</v>
       </c>
       <c r="J35" s="1"/>
@@ -3495,52 +3485,52 @@
     </row>
     <row r="36" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="137"/>
-      <c r="C36" s="141" t="s">
+      <c r="B36" s="80"/>
+      <c r="C36" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="108" t="s">
+      <c r="D36" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="128" t="s">
+      <c r="E36" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="F36" s="145" t="s">
+      <c r="F36" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="G36" s="153" t="s">
+      <c r="G36" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="H36" s="145" t="s">
+      <c r="H36" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="I36" s="118"/>
+      <c r="I36" s="46"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="137"/>
-      <c r="C37" s="142" t="s">
+      <c r="B37" s="80"/>
+      <c r="C37" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="108" t="s">
+      <c r="D37" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="106" t="s">
+      <c r="E37" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="146" t="s">
+      <c r="F37" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="G37" s="153" t="s">
+      <c r="G37" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="H37" s="145" t="s">
+      <c r="H37" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="I37" s="147" t="s">
+      <c r="I37" s="65" t="s">
         <v>191</v>
       </c>
       <c r="J37" s="1"/>
@@ -3549,26 +3539,26 @@
     </row>
     <row r="38" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="143"/>
-      <c r="C38" s="144" t="s">
+      <c r="B38" s="81"/>
+      <c r="C38" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="121" t="s">
+      <c r="D38" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="131" t="s">
+      <c r="E38" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="156" t="s">
+      <c r="F38" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="G38" s="157" t="s">
+      <c r="G38" s="75" t="s">
         <v>192</v>
       </c>
-      <c r="H38" s="156" t="s">
+      <c r="H38" s="74" t="s">
         <v>165</v>
       </c>
-      <c r="I38" s="158" t="s">
+      <c r="I38" s="76" t="s">
         <v>187</v>
       </c>
       <c r="J38" s="1"/>
@@ -3577,296 +3567,286 @@
     </row>
     <row r="39" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="103"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="111"/>
-      <c r="G39" s="112"/>
-      <c r="H39" s="111"/>
-      <c r="I39" s="114"/>
-      <c r="J39" s="113"/>
-      <c r="K39" s="113"/>
-      <c r="L39" s="113"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="109"/>
-      <c r="C40" s="103"/>
-      <c r="D40" s="109"/>
-      <c r="E40" s="110"/>
-      <c r="F40" s="111"/>
-      <c r="G40" s="112"/>
-      <c r="H40" s="111"/>
-      <c r="I40" s="112"/>
-      <c r="J40" s="113"/>
-      <c r="K40" s="113"/>
+      <c r="C40" s="5"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="103"/>
-      <c r="C41" s="103"/>
-      <c r="D41" s="109"/>
-      <c r="E41" s="110"/>
-      <c r="F41" s="111"/>
-      <c r="G41" s="112"/>
-      <c r="H41" s="111"/>
-      <c r="I41" s="112"/>
-      <c r="J41" s="113"/>
-      <c r="K41" s="113"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="103"/>
-      <c r="C42" s="104"/>
-      <c r="D42" s="109"/>
-      <c r="E42" s="110"/>
-      <c r="F42" s="111"/>
-      <c r="G42" s="112"/>
-      <c r="H42" s="111"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="113"/>
-      <c r="K42" s="113"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="36"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="103"/>
-      <c r="D43" s="109"/>
-      <c r="E43" s="110"/>
-      <c r="F43" s="111"/>
-      <c r="G43" s="112"/>
-      <c r="H43" s="111"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="113"/>
-      <c r="K43" s="113"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="103"/>
-      <c r="C44" s="103"/>
-      <c r="D44" s="105"/>
-      <c r="E44" s="110"/>
-      <c r="F44" s="111"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="111"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="113"/>
-      <c r="K44" s="113"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
     <row r="45" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="103"/>
-      <c r="C45" s="103"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="110"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="113"/>
-      <c r="K45" s="113"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="104"/>
-      <c r="D46" s="105"/>
-      <c r="E46" s="110"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="112"/>
-      <c r="H46" s="111"/>
-      <c r="I46" s="114"/>
-      <c r="J46" s="113"/>
-      <c r="K46" s="113"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
     <row r="47" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="103"/>
-      <c r="C47" s="103"/>
-      <c r="D47" s="105"/>
-      <c r="E47" s="114"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="112"/>
-      <c r="H47" s="111"/>
-      <c r="I47" s="114"/>
-      <c r="J47" s="113"/>
-      <c r="K47" s="113"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="103"/>
-      <c r="D48" s="105"/>
-      <c r="E48" s="110"/>
-      <c r="F48" s="111"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="111"/>
-      <c r="I48" s="114"/>
-      <c r="J48" s="113"/>
-      <c r="K48" s="113"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
     <row r="49" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="104"/>
-      <c r="C49" s="104"/>
-      <c r="D49" s="105"/>
-      <c r="E49" s="110"/>
-      <c r="F49" s="105"/>
-      <c r="G49" s="115"/>
-      <c r="H49" s="105"/>
-      <c r="I49" s="115"/>
-      <c r="J49" s="113"/>
-      <c r="K49" s="113"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="116"/>
-      <c r="C50" s="104"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="110"/>
-      <c r="F50" s="105"/>
-      <c r="G50" s="110"/>
-      <c r="H50" s="105"/>
-      <c r="I50" s="115"/>
-      <c r="J50" s="113"/>
-      <c r="K50" s="113"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="104"/>
-      <c r="D51" s="105"/>
-      <c r="E51" s="110"/>
-      <c r="F51" s="105"/>
-      <c r="G51" s="110"/>
-      <c r="H51" s="105"/>
-      <c r="I51" s="115"/>
-      <c r="J51" s="113"/>
-      <c r="K51" s="113"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="104"/>
-      <c r="D52" s="105"/>
-      <c r="E52" s="110"/>
-      <c r="F52" s="105"/>
-      <c r="G52" s="110"/>
-      <c r="H52" s="105"/>
-      <c r="I52" s="110"/>
-      <c r="J52" s="113"/>
-      <c r="K52" s="113"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
       <c r="L52" s="1"/>
     </row>
     <row r="53" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="104"/>
-      <c r="D53" s="105"/>
-      <c r="E53" s="110"/>
-      <c r="F53" s="105"/>
-      <c r="G53" s="110"/>
-      <c r="H53" s="105"/>
-      <c r="I53" s="110"/>
-      <c r="J53" s="113"/>
-      <c r="K53" s="113"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
       <c r="L53" s="1"/>
     </row>
     <row r="54" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="104"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="105"/>
-      <c r="E54" s="110"/>
-      <c r="F54" s="105"/>
-      <c r="G54" s="113"/>
-      <c r="H54" s="105"/>
-      <c r="I54" s="110"/>
-      <c r="J54" s="113"/>
-      <c r="K54" s="113"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
       <c r="L54" s="1"/>
     </row>
     <row r="55" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="B55" s="104"/>
-      <c r="C55" s="104"/>
-      <c r="D55" s="105"/>
-      <c r="E55" s="110"/>
-      <c r="F55" s="105"/>
-      <c r="G55" s="113"/>
-      <c r="H55" s="105"/>
-      <c r="I55" s="110"/>
-      <c r="J55" s="113"/>
-      <c r="K55" s="113"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
       <c r="L55" s="1"/>
     </row>
     <row r="56" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="104"/>
-      <c r="C56" s="104"/>
-      <c r="D56" s="105"/>
-      <c r="E56" s="110"/>
-      <c r="F56" s="105"/>
-      <c r="G56" s="113"/>
-      <c r="H56" s="105"/>
-      <c r="I56" s="110"/>
-      <c r="J56" s="113"/>
-      <c r="K56" s="113"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
       <c r="L56" s="1"/>
     </row>
     <row r="57" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="104"/>
-      <c r="C57" s="104"/>
-      <c r="D57" s="105"/>
-      <c r="E57" s="110"/>
-      <c r="F57" s="105"/>
-      <c r="G57" s="113"/>
-      <c r="H57" s="105"/>
-      <c r="I57" s="110"/>
-      <c r="J57" s="113"/>
-      <c r="K57" s="113"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
     <row r="58" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="104"/>
-      <c r="C58" s="104"/>
-      <c r="D58" s="105"/>
-      <c r="E58" s="110"/>
-      <c r="F58" s="105"/>
-      <c r="G58" s="113"/>
-      <c r="H58" s="105"/>
-      <c r="I58" s="110"/>
-      <c r="J58" s="113"/>
-      <c r="K58" s="113"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="104"/>
-      <c r="C59" s="104"/>
-      <c r="D59" s="105"/>
-      <c r="E59" s="117"/>
-      <c r="F59" s="105"/>
-      <c r="G59" s="113"/>
-      <c r="H59" s="105"/>
-      <c r="I59" s="110"/>
-      <c r="J59" s="113"/>
-      <c r="K59" s="113"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
       <c r="L59" s="1"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13431,11 +13411,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C19:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B16:B38"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="H2:I6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:G6"/>
@@ -13444,6 +13419,11 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C19:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B16:B38"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
@@ -13460,8 +13440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:L988"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13476,44 +13456,44 @@
   <sheetData>
     <row r="1" spans="2:12" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="90" t="s">
+      <c r="B2" s="145"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="151" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="53" t="s">
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="117" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="54"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="118"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="86"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="54"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="152"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="118"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="88"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="55"/>
+      <c r="B5" s="149"/>
+      <c r="C5" s="150"/>
+      <c r="D5" s="153"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="153"/>
+      <c r="H5" s="119"/>
       <c r="L5" s="5" t="s">
         <v>1</v>
       </c>
@@ -13531,15 +13511,15 @@
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="2:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="76"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="137"/>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
@@ -13548,12 +13528,12 @@
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="138" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="79"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="140"/>
       <c r="H8" s="6" t="s">
         <v>9</v>
       </c>
@@ -13565,12 +13545,12 @@
       <c r="C9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="82"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="143"/>
       <c r="H9" s="22" t="s">
         <v>10</v>
       </c>
@@ -13582,13 +13562,13 @@
       <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="134" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="72" t="s">
+      <c r="E10" s="115"/>
+      <c r="F10" s="115"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="133" t="s">
         <v>11</v>
       </c>
     </row>
@@ -13599,13 +13579,13 @@
       <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="71"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="144"/>
+      <c r="H11" s="132"/>
     </row>
     <row r="12" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
@@ -13614,13 +13594,13 @@
       <c r="C12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="61" t="s">
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="124" t="s">
         <v>12</v>
       </c>
     </row>
@@ -13631,13 +13611,13 @@
       <c r="C13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="94"/>
-      <c r="H13" s="71"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="132"/>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
@@ -13646,12 +13626,12 @@
       <c r="C14" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="58"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="116"/>
       <c r="H14" s="21" t="s">
         <v>13</v>
       </c>
@@ -13663,13 +13643,13 @@
       <c r="C15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="131" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="61" t="s">
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="124" t="s">
         <v>14</v>
       </c>
     </row>
@@ -13680,13 +13660,13 @@
       <c r="C16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="62"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="125"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
@@ -13695,12 +13675,12 @@
       <c r="C17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="116"/>
       <c r="H17" s="17" t="s">
         <v>15</v>
       </c>
@@ -13712,12 +13692,12 @@
       <c r="C18" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="127"/>
       <c r="H18" s="24" t="s">
         <v>16</v>
       </c>
@@ -13729,12 +13709,12 @@
       <c r="C19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="59" t="s">
+      <c r="D19" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="36"/>
+      <c r="E19" s="122"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="123"/>
       <c r="H19" s="23" t="s">
         <v>17</v>
       </c>
@@ -17068,16 +17048,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D15:G15"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D15:G15"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="D10:G10"/>

</xml_diff>